<commit_message>
End of class Thurs
</commit_message>
<xml_diff>
--- a/Population.xlsx
+++ b/Population.xlsx
@@ -248,10 +248,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +590,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +619,7 @@
       <c r="C2" s="1">
         <v>582549</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>739.02</v>
       </c>
     </row>
@@ -634,7 +633,7 @@
       <c r="C3" s="1">
         <v>1760</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>738.33</v>
       </c>
     </row>
@@ -648,7 +647,7 @@
       <c r="C4" s="1">
         <v>18032</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>594.58000000000004</v>
       </c>
     </row>
@@ -662,7 +661,7 @@
       <c r="C5" s="1">
         <v>95835</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1636.46</v>
       </c>
     </row>
@@ -676,7 +675,7 @@
       <c r="C6" s="1">
         <v>27925</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>1020.01</v>
       </c>
     </row>
@@ -690,7 +689,7 @@
       <c r="C7" s="1">
         <v>7883</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1150.73</v>
       </c>
     </row>
@@ -704,7 +703,7 @@
       <c r="C8" s="1">
         <v>400263</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>715.94</v>
       </c>
     </row>
@@ -718,7 +717,7 @@
       <c r="C9" s="1">
         <v>11186</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1006.37</v>
       </c>
     </row>
@@ -732,7 +731,7 @@
       <c r="C10" s="1">
         <v>88159</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1707.88</v>
       </c>
     </row>
@@ -746,7 +745,7 @@
       <c r="C11" s="1">
         <v>315531</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>5957.99</v>
       </c>
     </row>
@@ -760,7 +759,7 @@
       <c r="C12" s="1">
         <v>10778</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1313.95</v>
       </c>
     </row>
@@ -774,7 +773,7 @@
       <c r="C13" s="1">
         <v>61559</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>3567.99</v>
       </c>
     </row>
@@ -788,7 +787,7 @@
       <c r="C14" s="1">
         <v>56067</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>4176.6000000000004</v>
       </c>
     </row>
@@ -802,7 +801,7 @@
       <c r="C15" s="1">
         <v>9478</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>10180.879999999999</v>
       </c>
     </row>
@@ -816,7 +815,7 @@
       <c r="C16" s="1">
         <v>284367</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>8131.92</v>
       </c>
     </row>
@@ -830,7 +829,7 @@
       <c r="C17" s="1">
         <v>43867</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>1389.42</v>
       </c>
     </row>
@@ -844,7 +843,7 @@
       <c r="C18" s="1">
         <v>35492</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>1256.46</v>
       </c>
     </row>
@@ -858,7 +857,7 @@
       <c r="C19" s="1">
         <v>12710</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>4541.18</v>
       </c>
     </row>
@@ -872,7 +871,7 @@
       <c r="C20" s="1">
         <v>3445076</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>4057.88</v>
       </c>
     </row>
@@ -886,7 +885,7 @@
       <c r="C21" s="1">
         <v>49140</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>2137.0700000000002</v>
       </c>
     </row>
@@ -900,7 +899,7 @@
       <c r="C22" s="1">
         <v>111214</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>520.30999999999995</v>
       </c>
     </row>
@@ -914,7 +913,7 @@
       <c r="C23" s="1">
         <v>10188</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>1448.82</v>
       </c>
     </row>
@@ -928,7 +927,7 @@
       <c r="C24" s="1">
         <v>40323</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>3506.34</v>
       </c>
     </row>
@@ -942,7 +941,7 @@
       <c r="C25" s="1">
         <v>83698</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>1934.97</v>
       </c>
     </row>
@@ -956,7 +955,7 @@
       <c r="C26" s="1">
         <v>5192</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>3917.77</v>
       </c>
     </row>
@@ -970,7 +969,7 @@
       <c r="C27" s="1">
         <v>13912</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>3048.98</v>
       </c>
     </row>
@@ -984,7 +983,7 @@
       <c r="C28" s="1">
         <v>139048</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>3280.6</v>
       </c>
     </row>
@@ -998,7 +997,7 @@
       <c r="C29" s="1">
         <v>54759</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>748.36</v>
       </c>
     </row>
@@ -1012,7 +1011,7 @@
       <c r="C30" s="1">
         <v>52590</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>957.77</v>
       </c>
     </row>
@@ -1026,7 +1025,7 @@
       <c r="C31" s="1">
         <v>1048907</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>790.57</v>
       </c>
     </row>
@@ -1040,7 +1039,7 @@
       <c r="C32" s="1">
         <v>152648</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>1407.01</v>
       </c>
     </row>
@@ -1054,7 +1053,7 @@
       <c r="C33" s="1">
         <v>15566</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>2553.04</v>
       </c>
     </row>
@@ -1068,7 +1067,7 @@
       <c r="C34" s="1">
         <v>800707</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>7206.48</v>
       </c>
     </row>
@@ -1082,7 +1081,7 @@
       <c r="C35" s="1">
         <v>555932</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>964.64</v>
       </c>
     </row>
@@ -1096,7 +1095,7 @@
       <c r="C36" s="1">
         <v>17870</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>1388.71</v>
       </c>
     </row>
@@ -1110,7 +1109,7 @@
       <c r="C37" s="1">
         <v>699637</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <v>20056.939999999999</v>
       </c>
     </row>
@@ -1124,7 +1123,7 @@
       <c r="C38" s="1">
         <v>1164786</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>4206.63</v>
       </c>
     </row>
@@ -1138,7 +1137,7 @@
       <c r="C39" s="1">
         <v>376942</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>46.87</v>
       </c>
     </row>
@@ -1152,7 +1151,7 @@
       <c r="C40" s="1">
         <v>233755</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>1391.32</v>
       </c>
     </row>
@@ -1166,7 +1165,7 @@
       <c r="C41" s="1">
         <v>117315</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>3298.57</v>
       </c>
     </row>
@@ -1180,7 +1179,7 @@
       <c r="C42" s="1">
         <v>271031</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>448.41</v>
       </c>
     </row>
@@ -1194,7 +1193,7 @@
       <c r="C43" s="1">
         <v>152834</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>2735.09</v>
       </c>
     </row>
@@ -1208,7 +1207,7 @@
       <c r="C44" s="1">
         <v>631920</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>1290.0999999999999</v>
       </c>
     </row>
@@ -1222,7 +1221,7 @@
       <c r="C45" s="1">
         <v>104476</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>445.17</v>
       </c>
     </row>
@@ -1236,7 +1235,7 @@
       <c r="C46" s="1">
         <v>77313</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>3775.4</v>
       </c>
     </row>
@@ -1250,7 +1249,7 @@
       <c r="C47" s="1">
         <v>2328</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>953.21</v>
       </c>
     </row>
@@ -1264,7 +1263,7 @@
       <c r="C48" s="1">
         <v>23910</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>6277.89</v>
       </c>
     </row>
@@ -1278,7 +1277,7 @@
       <c r="C49" s="1">
         <v>152698</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>821.76</v>
       </c>
     </row>
@@ -1292,7 +1291,7 @@
       <c r="C50" s="1">
         <v>204572</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="1">
         <v>1575.85</v>
       </c>
     </row>
@@ -1306,7 +1305,7 @@
       <c r="C51" s="1">
         <v>179503</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="1">
         <v>1494.83</v>
       </c>
     </row>
@@ -1320,7 +1319,7 @@
       <c r="C52" s="1">
         <v>33858</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>602.41</v>
       </c>
     </row>
@@ -1334,7 +1333,7 @@
       <c r="C53" s="1">
         <v>26987</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="1">
         <v>2949.71</v>
       </c>
     </row>
@@ -1348,7 +1347,7 @@
       <c r="C54" s="1">
         <v>8681</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <v>3179.25</v>
       </c>
     </row>
@@ -1362,7 +1361,7 @@
       <c r="C55" s="1">
         <v>141696</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <v>4824.21</v>
       </c>
     </row>
@@ -1376,7 +1375,7 @@
       <c r="C56" s="1">
         <v>31244</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="1">
         <v>2220.88</v>
       </c>
     </row>
@@ -1390,7 +1389,7 @@
       <c r="C57" s="1">
         <v>281695</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="1">
         <v>1843.13</v>
       </c>
     </row>
@@ -1404,7 +1403,7 @@
       <c r="C58" s="1">
         <v>75054</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>1014.69</v>
       </c>
     </row>
@@ -1418,7 +1417,7 @@
       <c r="C59" s="1">
         <v>27635</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>631.84</v>
       </c>
     </row>

</xml_diff>